<commit_message>
added test with only area changing continuously through the two truss bars
</commit_message>
<xml_diff>
--- a/Data/BatchTestTruss.xlsx
+++ b/Data/BatchTestTruss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\del\Desktop\SSOToolboxGitlab\sso-toolbox\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744529C9-CCC6-4CC8-810A-E0FFDB550EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0A5D3E-7495-4F75-8D0F-C924047135A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Number Samples Per Iteration</t>
   </si>
   <si>
-    <t>Max Iter</t>
-  </si>
-  <si>
     <t>Candidate Space Constructor</t>
   </si>
   <si>
@@ -103,6 +100,21 @@
   </si>
   <si>
     <t>S015</t>
+  </si>
+  <si>
+    <t>S016</t>
+  </si>
+  <si>
+    <t>S017</t>
+  </si>
+  <si>
+    <t>S018</t>
+  </si>
+  <si>
+    <t>S019</t>
+  </si>
+  <si>
+    <t>S020</t>
   </si>
 </sst>
 </file>
@@ -158,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -181,29 +193,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -485,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,12 +495,11 @@
     <col min="1" max="1" width="8.08984375" customWidth="1"/>
     <col min="2" max="2" width="12.81640625" customWidth="1"/>
     <col min="3" max="3" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -517,11 +515,8 @@
       <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -529,19 +524,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="1">
-        <v>400</v>
-      </c>
-      <c r="D2" s="1">
-        <v>300</v>
+        <v>100</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -549,19 +541,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>500</v>
-      </c>
-      <c r="D3" s="1">
-        <v>300</v>
+        <v>200</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -569,262 +558,303 @@
         <v>1</v>
       </c>
       <c r="C4" s="2">
+        <v>300</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>400</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>500</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
         <v>600</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>700</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>800</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>900</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2">
+        <v>200</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2">
         <v>300</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2">
+        <v>400</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
+        <v>500</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2">
+        <v>600</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2">
         <v>700</v>
       </c>
-      <c r="D5" s="1">
-        <v>300</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2">
         <v>800</v>
       </c>
-      <c r="D6" s="1">
-        <v>300</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="2">
         <v>900</v>
       </c>
-      <c r="D7" s="1">
-        <v>300</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1">
-        <v>100</v>
-      </c>
-      <c r="D8" s="1">
-        <v>300</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2">
-        <v>200</v>
-      </c>
-      <c r="D9" s="1">
-        <v>300</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="5">
-        <v>300</v>
-      </c>
-      <c r="D10" s="1">
-        <v>300</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="5">
-        <v>400</v>
-      </c>
-      <c r="D11" s="1">
-        <v>300</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="5">
-        <v>500</v>
-      </c>
-      <c r="D12" s="1">
-        <v>300</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="5">
-        <v>600</v>
-      </c>
-      <c r="D13" s="1">
-        <v>300</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5">
-        <v>700</v>
-      </c>
-      <c r="D14" s="1">
-        <v>300</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="5">
-        <v>800</v>
-      </c>
-      <c r="D15" s="1">
-        <v>300</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="5">
-        <v>900</v>
-      </c>
-      <c r="D16" s="1">
-        <v>300</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>